<commit_message>
I updated Chale Proposal 2
</commit_message>
<xml_diff>
--- a/inst/lectures/student_folders/chale/Proposal 2.xlsx
+++ b/inst/lectures/student_folders/chale/Proposal 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="187" windowWidth="12007" windowHeight="2487"/>
+    <workbookView xWindow="0" yWindow="280" windowWidth="12007" windowHeight="2487"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Recommend an analysis technique:</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Can Wait until v2.0?</t>
   </si>
   <si>
-    <t>50%. Computes performance metrics in Python but retuculate does not return object to R</t>
-  </si>
-  <si>
     <t>CSV data file</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
   </si>
   <si>
     <t>Data frame and visual plots of Recall, runtime, pareto efficients</t>
-  </si>
-  <si>
-    <t>Python only</t>
   </si>
   <si>
     <t>window to choose.file &amp; choose.directory so save results</t>
@@ -461,7 +455,7 @@
   <dimension ref="B4:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -476,10 +470,10 @@
   <sheetData>
     <row r="4" spans="2:10" ht="43" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -520,21 +514,21 @@
         <v>50</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="43" x14ac:dyDescent="0.5">
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -549,16 +543,16 @@
         <v>25</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="75" customHeight="1" x14ac:dyDescent="0.5">
@@ -571,23 +565,23 @@
       <c r="D7" s="4">
         <v>3</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>14</v>
+      <c r="E7" s="6">
+        <v>1</v>
       </c>
       <c r="F7" s="4">
         <v>20</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="71.7" x14ac:dyDescent="0.5">
@@ -607,16 +601,16 @@
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>